<commit_message>
added test cases and test models
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/01_ARE startup/Test_cases_ARE_startup.xlsx
+++ b/Tests/integrationTests/01_ARE startup/Test_cases_ARE_startup.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Number</t>
   </si>
@@ -230,12 +230,24 @@
   <si>
     <t>ARE should start with the model running and  show up informative error message</t>
   </si>
+  <si>
+    <t>Test Execution Infos</t>
+  </si>
+  <si>
+    <t>Name of Tester:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Environment (OS + Version, Architecture, Java Version):</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +274,14 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -311,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -326,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,7 +630,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +654,12 @@
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
@@ -639,9 +668,15 @@
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="D3" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
+      <c r="D4" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">

</xml_diff>

<commit_message>
updated tests: use start.bat for testing instead of Are.exe because start.bat is now without console window and does not need an installed .NET framework
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/01_ARE startup/Test_cases_ARE_startup.xlsx
+++ b/Tests/integrationTests/01_ARE startup/Test_cases_ARE_startup.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Number</t>
   </si>
@@ -190,14 +190,6 @@
     <t>ARE start file: start.bat (start.sh - Linux)</t>
   </si>
   <si>
-    <t>ARE start file: Are.exe (start.sh - Linux)
-model file: ARE startup/autostart_damaged.acs</t>
-  </si>
-  <si>
-    <t>ARE start file: Are.exe (start.sh - Linux)
-ARE startup/Ergo-Kopf-Musik-einfach_v2.5.acs</t>
-  </si>
-  <si>
     <t>Use old model file Ergo-Kopf-Musik-einfach_v2.5.acs (not up 2 date with bundle_descriptors of used plugins)</t>
   </si>
   <si>
@@ -215,10 +207,6 @@
   </si>
   <si>
     <t>Use old model file GamepadMouse.acs (without plugging in Gamepad)</t>
-  </si>
-  <si>
-    <t>ARE start file: Are.exe (start.sh - Linux)
-ARE startup/GamepadMouse.acs</t>
   </si>
   <si>
     <t>1. Backup original model file models/autostart.xml
@@ -241,6 +229,22 @@
   </si>
   <si>
     <t>Environment (OS + Version, Architecture, Java Version):</t>
+  </si>
+  <si>
+    <t>ARE start file: start.bat (start.sh - Linux)
+model file: ARE startup/autostart_damaged.acs</t>
+  </si>
+  <si>
+    <t>ARE start file: start.bat (start.sh - Linux)
+ARE startup/Ergo-Kopf-Musik-einfach_v2.5.acs</t>
+  </si>
+  <si>
+    <t>ARE start file: start.bat (start.sh - Linux)
+ARE startup/GamepadMouse.acs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This test may fail, because Are.exe depends on an intalled .NET framework which is optonal for downstripped installation files. 
+ARE should start with standard demo model </t>
   </si>
 </sst>
 </file>
@@ -619,7 +623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,7 +634,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,10 +659,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
@@ -666,16 +670,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="D4" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -748,7 +752,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -760,10 +764,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
@@ -775,13 +779,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>18</v>
@@ -790,19 +794,19 @@
     </row>
     <row r="12" spans="1:6" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="F12" s="5"/>
     </row>

</xml_diff>